<commit_message>
data(xlsx): < dice-report width field-names/del units, fix 'vehile' typo
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17571"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\compas.vinz\co2mpas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Home\ankostis\Work\co2mpas.git\co2mpas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="5" r:id="rId1"/>
     <sheet name="dice_report" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="53">
   <si>
     <t>Vehicle H</t>
   </si>
@@ -36,34 +36,7 @@
     <t>units</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>cc</t>
-  </si>
-  <si>
-    <t>alternator_model score</t>
-  </si>
-  <si>
-    <t>at_model score</t>
-  </si>
-  <si>
-    <t>clutch_torque_converter_model score</t>
-  </si>
-  <si>
-    <t>co2_params score</t>
-  </si>
-  <si>
-    <t>engine_cold_start_speed_model score</t>
-  </si>
-  <si>
-    <t>engine_coolant_temperature_model score</t>
-  </si>
-  <si>
-    <t>engine_speed_model score</t>
-  </si>
-  <si>
-    <t>start_stop_model score</t>
   </si>
   <si>
     <t xml:space="preserve">CO2MPAS deviation </t>
@@ -268,19 +241,43 @@
     <t>Model scores</t>
   </si>
   <si>
-    <t>Vehile</t>
-  </si>
-  <si>
     <t>Vehicle</t>
   </si>
   <si>
     <t xml:space="preserve">CO2MPAS_deviation </t>
+  </si>
+  <si>
+    <t>at_model</t>
+  </si>
+  <si>
+    <t>alternator_model</t>
+  </si>
+  <si>
+    <t>clutch_torque_converter_model</t>
+  </si>
+  <si>
+    <t>co2_params</t>
+  </si>
+  <si>
+    <t>engine_cold_start_speed_model</t>
+  </si>
+  <si>
+    <t>engine_coolant_temperature_model</t>
+  </si>
+  <si>
+    <t>engine_speed_model</t>
+  </si>
+  <si>
+    <t>start_stop_model</t>
+  </si>
+  <si>
+    <t>Model_scores</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -423,7 +420,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -527,10 +524,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -542,21 +535,7 @@
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <fill>
         <patternFill>
@@ -885,22 +864,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E48"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.28515625" style="5"/>
+    <col min="4" max="4" width="10.1796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.26953125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="e">
         <f ca="1">INDIRECT("summary!_info_vehicle_family_id_Value")</f>
@@ -909,9 +890,9 @@
       <c r="C1" s="3"/>
       <c r="D1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2" t="e">
         <f ca="1">INDIRECT("summary!_info_CO2MPAS_version_Value")</f>
@@ -920,9 +901,9 @@
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2" t="e">
         <f ca="1">INDIRECT("summary!_info_Simulation_started_Value")</f>
@@ -931,9 +912,9 @@
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B4" s="6" t="e">
         <f ca="1">INDIRECT("summary!_info_type_approval_mode_Value")</f>
@@ -942,21 +923,21 @@
       <c r="C4" s="3"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="3"/>
       <c r="D5" s="7"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="3"/>
       <c r="D6" s="7"/>
     </row>
-    <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="B7" s="22" t="s">
         <v>0</v>
@@ -968,9 +949,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="B8" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_")</f>
@@ -981,12 +962,12 @@
         <v>#REF!</v>
       </c>
       <c r="D8" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="B9" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_")</f>
@@ -997,12 +978,12 @@
         <v>#REF!</v>
       </c>
       <c r="D9" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="24" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B10" s="24" t="e">
         <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100</f>
@@ -1013,26 +994,26 @@
         <v>#REF!</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="13"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="14"/>
       <c r="C12" s="3"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="B13" s="22" t="s">
         <v>0</v>
@@ -1044,9 +1025,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B14" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_")</f>
@@ -1057,12 +1038,12 @@
         <v>#REF!</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="B15" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_")</f>
@@ -1073,12 +1054,12 @@
         <v>#REF!</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B16" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_")</f>
@@ -1089,38 +1070,38 @@
         <v>#REF!</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="20"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="B18" s="14"/>
       <c r="C18" s="3"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D19" s="22" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B20" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score")</f>
@@ -1130,13 +1111,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D20" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D20" s="23"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B21" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score")</f>
@@ -1146,13 +1125,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D21" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D21" s="23"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B22" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score")</f>
@@ -1162,13 +1139,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D22" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22" s="23"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B23" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score")</f>
@@ -1178,13 +1153,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D23" s="23"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B24" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score")</f>
@@ -1194,13 +1167,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D24" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D24" s="23"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B25" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score")</f>
@@ -1210,13 +1181,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D25" s="28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="27"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B26" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score")</f>
@@ -1226,13 +1195,11 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D26" s="23"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B27" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score")</f>
@@ -1242,39 +1209,37 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D27" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D27" s="23"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="B28" s="14"/>
       <c r="C28" s="3"/>
       <c r="D28" s="7"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="B29" s="14"/>
       <c r="C29" s="3"/>
       <c r="D29" s="7"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D30" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B31" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__")</f>
@@ -1284,13 +1249,11 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__")</f>
         <v>#REF!</v>
       </c>
-      <c r="D31" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D31" s="23"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" s="16" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B32" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_")</f>
@@ -1301,12 +1264,12 @@
         <v>#REF!</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" s="16" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B33" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__")</f>
@@ -1316,13 +1279,11 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__")</f>
         <v>#REF!</v>
       </c>
-      <c r="D33" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D33" s="23"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" s="16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B34" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__")</f>
@@ -1332,13 +1293,11 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__")</f>
         <v>#REF!</v>
       </c>
-      <c r="D34" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34" s="23"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>0</v>
@@ -1350,9 +1309,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B36" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_")</f>
@@ -1363,12 +1322,12 @@
         <v>#REF!</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" s="17" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B37" s="18" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__")</f>
@@ -1379,12 +1338,12 @@
         <v>#REF!</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A38" s="17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B38" s="18" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_")</f>
@@ -1395,12 +1354,12 @@
         <v>#REF!</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" s="16" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B39" s="19" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_")</f>
@@ -1411,12 +1370,12 @@
         <v>#REF!</v>
       </c>
       <c r="D39" s="25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>0</v>
@@ -1428,9 +1387,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" s="16" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B41" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_")</f>
@@ -1441,12 +1400,12 @@
         <v>#REF!</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B42" s="18" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__")</f>
@@ -1457,12 +1416,12 @@
         <v>#REF!</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="16.5" x14ac:dyDescent="0.35">
       <c r="A43" s="17" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B43" s="18" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_")</f>
@@ -1473,12 +1432,12 @@
         <v>#REF!</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" s="16" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="B44" s="19" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_")</f>
@@ -1489,12 +1448,12 @@
         <v>#REF!</v>
       </c>
       <c r="D44" s="25" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" s="16" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B45" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_")</f>
@@ -1505,12 +1464,12 @@
         <v>#REF!</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="16" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="B46" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_")</f>
@@ -1521,12 +1480,12 @@
         <v>#REF!</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" s="16" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B47" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_")</f>
@@ -1537,12 +1496,12 @@
         <v>#REF!</v>
       </c>
       <c r="D47" s="25" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" s="16" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B48" s="10" t="e">
         <f ca="1">INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_")</f>
@@ -1553,7 +1512,7 @@
         <v>#REF!</v>
       </c>
       <c r="D48" s="25" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1572,10 +1531,10 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="5" priority="11">
+    <cfRule type="expression" dxfId="3" priority="11">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="12">
+    <cfRule type="expression" dxfId="2" priority="12">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1618,80 +1577,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.81640625" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.81640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.453125" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.85546875" style="9"/>
+    <col min="4" max="16384" width="11.81640625" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="22" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B2" s="2" t="e">
         <f ca="1">INDIRECT("summary!_info_vehicle_family_id_Value")</f>
         <v>#REF!</v>
       </c>
       <c r="C2" s="26"/>
-      <c r="D2" s="27"/>
-    </row>
-    <row r="3" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="e">
         <f ca="1">INDIRECT("summary!_info_CO2MPAS_version_Value")</f>
         <v>#REF!</v>
       </c>
       <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-    </row>
-    <row r="4" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B4" s="2" t="e">
         <f ca="1">INDIRECT("summary!_info_Simulation_started_Value")</f>
         <v>#REF!</v>
       </c>
       <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-    </row>
-    <row r="5" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B5" s="6" t="e">
         <f ca="1">INDIRECT("summary!_info_type_approval_mode_Value")</f>
         <v>#REF!</v>
       </c>
       <c r="C5" s="26"/>
-      <c r="D5" s="23"/>
-    </row>
-    <row r="6" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B6" s="24" t="e">
         <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100</f>
@@ -1701,27 +1652,21 @@
         <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="24" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A8" s="16" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B8" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__")</f>
@@ -1731,13 +1676,10 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__")</f>
         <v>#REF!</v>
       </c>
-      <c r="D8" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A9" s="16" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B9" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_")</f>
@@ -1747,13 +1689,10 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_")</f>
         <v>#REF!</v>
       </c>
-      <c r="D9" s="23" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A10" s="16" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B10" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__")</f>
@@ -1763,13 +1702,10 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__")</f>
         <v>#REF!</v>
       </c>
-      <c r="D10" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A11" s="16" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B11" s="8" t="e">
         <f ca="1">INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__")</f>
@@ -1779,27 +1715,21 @@
         <f ca="1">INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__")</f>
         <v>#REF!</v>
       </c>
-      <c r="D11" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="B13" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score")</f>
@@ -1809,13 +1739,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D13" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
-        <v>6</v>
+        <v>44</v>
       </c>
       <c r="B14" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score")</f>
@@ -1825,13 +1752,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D14" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B15" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score")</f>
@@ -1841,13 +1765,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D15" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="B16" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score")</f>
@@ -1857,13 +1778,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D16" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B17" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score")</f>
@@ -1873,13 +1791,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D17" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="5" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="B18" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score")</f>
@@ -1889,13 +1804,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D18" s="28" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="B19" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score")</f>
@@ -1905,13 +1817,10 @@
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_l_score")</f>
         <v>#REF!</v>
       </c>
-      <c r="D19" s="23" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="B20" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score")</f>
@@ -1920,9 +1829,6 @@
       <c r="C20" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_l_score")</f>
         <v>#REF!</v>
-      </c>
-      <c r="D20" s="23" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -1941,27 +1847,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5">
-    <cfRule type="expression" dxfId="3" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>$B$5="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="12">
+    <cfRule type="expression" dxfId="0" priority="12">
       <formula>$B$5="True"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
     <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="-4"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="4"/>
-        <color rgb="FFFFC000"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D6">
-    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
data(xlsx): del extra space in CO2MPASS_deviation label
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="28800" windowHeight="16260" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="5" r:id="rId1"/>
@@ -244,9 +244,6 @@
     <t>Vehicle</t>
   </si>
   <si>
-    <t xml:space="preserve">CO2MPAS_deviation </t>
-  </si>
-  <si>
     <t>at_model</t>
   </si>
   <si>
@@ -272,6 +269,9 @@
   </si>
   <si>
     <t>Model_scores</t>
+  </si>
+  <si>
+    <t>CO2MPAS_deviation</t>
   </si>
 </sst>
 </file>
@@ -866,7 +866,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B20" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score")</f>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score")</f>
@@ -1129,7 +1129,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B22" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score")</f>
@@ -1143,7 +1143,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B23" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score")</f>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B24" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score")</f>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B25" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score")</f>
@@ -1185,7 +1185,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B26" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score")</f>
@@ -1199,7 +1199,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score")</f>
@@ -1579,7 +1579,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.81640625" defaultRowHeight="12" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1642,7 +1644,7 @@
     </row>
     <row r="6" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A6" s="24" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B6" s="24" t="e">
         <f ca="1">(INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100</f>
@@ -1718,7 +1720,7 @@
     </row>
     <row r="12" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="22" t="s">
         <v>31</v>
@@ -1729,7 +1731,7 @@
     </row>
     <row r="13" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A13" s="16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score")</f>
@@ -1742,7 +1744,7 @@
     </row>
     <row r="14" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A14" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score")</f>
@@ -1755,7 +1757,7 @@
     </row>
     <row r="15" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A15" s="16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B15" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score")</f>
@@ -1768,7 +1770,7 @@
     </row>
     <row r="16" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A16" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B16" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score")</f>
@@ -1781,7 +1783,7 @@
     </row>
     <row r="17" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A17" s="16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B17" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score")</f>
@@ -1794,7 +1796,7 @@
     </row>
     <row r="18" spans="1:3" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A18" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B18" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score")</f>
@@ -1807,7 +1809,7 @@
     </row>
     <row r="19" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A19" s="16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score")</f>
@@ -1820,7 +1822,7 @@
     </row>
     <row r="20" spans="1:3" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A20" s="16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B20" s="8" t="e">
         <f ca="1">INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score")</f>

</xml_diff>

<commit_message>
data(xlsx): HIDE DICE SHEET on out-template + del duplicate deviation
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="6" r:id="rId1"/>
-    <sheet name="dice_report" sheetId="4" r:id="rId2"/>
+    <sheet name="dice_report" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
     <t>Vehicle H</t>
   </si>
@@ -752,7 +752,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -967,18 +967,6 @@
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="2" fontId="9" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1332,9 +1320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>
@@ -2137,21 +2123,11 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="7"/>
     </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A31" s="55" t="s">
-        <v>4</v>
-      </c>
-      <c r="B31" s="56" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
-        <v/>
-      </c>
-      <c r="C31" s="57" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100,"")</f>
-        <v/>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>5</v>
-      </c>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1">
+      <c r="A31" s="4"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
@@ -2167,9 +2143,15 @@
       <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A32" s="4"/>
-      <c r="B32" s="14"/>
-      <c r="C32" s="3"/>
+      <c r="A32" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>1</v>
+      </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -2186,16 +2168,20 @@
       <c r="Q32" s="7"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A33" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" s="7"/>
+      <c r="A33" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B33" s="10" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
+        <v/>
+      </c>
+      <c r="C33" s="10" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
+        <v/>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
       <c r="G33" s="7"/>
@@ -2211,19 +2197,19 @@
       <c r="Q33" s="7"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A34" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B34" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
-        <v/>
-      </c>
-      <c r="C34" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
+      <c r="A34" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B34" s="18" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
+        <v/>
+      </c>
+      <c r="C34" s="18" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="D34" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2241,18 +2227,18 @@
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1">
       <c r="A35" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B35" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="C35" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="D35" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2269,19 +2255,19 @@
       <c r="Q35" s="7"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A36" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B36" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
-        <v/>
-      </c>
-      <c r="C36" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
-        <v/>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>21</v>
+      <c r="A36" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="19" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="C36" s="19" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>23</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2298,20 +2284,16 @@
       <c r="Q36" s="7"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A37" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="19" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
-        <v/>
-      </c>
-      <c r="C37" s="19" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
-        <v/>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>23</v>
-      </c>
+      <c r="A37" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
@@ -2327,16 +2309,20 @@
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A38" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C38" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="7"/>
+      <c r="A38" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B38" s="10" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
+        <v/>
+      </c>
+      <c r="C38" s="10" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
+        <v/>
+      </c>
+      <c r="D38" s="7" t="s">
+        <v>17</v>
+      </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
       <c r="G38" s="7"/>
@@ -2352,19 +2338,19 @@
       <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A39" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
-        <v/>
-      </c>
-      <c r="C39" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
+      <c r="A39" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="18" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
+        <v/>
+      </c>
+      <c r="C39" s="18" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="D39" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2382,18 +2368,18 @@
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1">
       <c r="A40" s="17" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B40" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="C40" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="D40" s="7" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2410,19 +2396,19 @@
       <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A41" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B41" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
-        <v/>
-      </c>
-      <c r="C41" s="18" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
-        <v/>
-      </c>
-      <c r="D41" s="7" t="s">
-        <v>21</v>
+      <c r="A41" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B41" s="19" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="C41" s="19" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
+        <v/>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>23</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2440,18 +2426,18 @@
     </row>
     <row r="42" spans="1:17" ht="15.75" customHeight="1">
       <c r="A42" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B42" s="19" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
-        <v/>
-      </c>
-      <c r="C42" s="19" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
+        <v>26</v>
+      </c>
+      <c r="B42" s="10" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
+        <v/>
+      </c>
+      <c r="C42" s="10" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D42" s="41" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -2469,14 +2455,14 @@
     </row>
     <row r="43" spans="1:17" ht="15.75" customHeight="1">
       <c r="A43" s="16" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B43" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="C43" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D43" s="41" t="s">
@@ -2498,14 +2484,14 @@
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1">
       <c r="A44" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B44" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="C44" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D44" s="41" t="s">
@@ -2527,14 +2513,14 @@
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1">
       <c r="A45" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B45" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="C45" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
+        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D45" s="41" t="s">
@@ -2554,29 +2540,19 @@
       <c r="P45" s="7"/>
       <c r="Q45" s="7"/>
     </row>
-    <row r="46" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A46" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B46" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
-        <v/>
-      </c>
-      <c r="C46" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
-        <v/>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="7"/>
-      <c r="F46" s="7"/>
-      <c r="G46" s="7"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="7"/>
-      <c r="K46" s="7"/>
-      <c r="L46" s="7"/>
+    <row r="46" spans="1:17" hidden="1">
+      <c r="A46" s="3"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
       <c r="M46" s="7"/>
       <c r="N46" s="7"/>
       <c r="O46" s="7"/>
@@ -2604,17 +2580,17 @@
     </row>
     <row r="48" spans="1:17" hidden="1">
       <c r="A48" s="3"/>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4"/>
-      <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="3"/>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
       <c r="M48" s="7"/>
       <c r="N48" s="7"/>
       <c r="O48" s="7"/>
@@ -2622,18 +2598,18 @@
       <c r="Q48" s="7"/>
     </row>
     <row r="49" spans="1:17" hidden="1">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7"/>
+      <c r="G49" s="7"/>
+      <c r="H49" s="7"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
       <c r="M49" s="7"/>
       <c r="N49" s="7"/>
       <c r="O49" s="7"/>
@@ -2641,7 +2617,7 @@
       <c r="Q49" s="7"/>
     </row>
     <row r="50" spans="1:17" hidden="1">
-      <c r="A50" s="7"/>
+      <c r="A50" s="3"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -2755,7 +2731,7 @@
       <c r="Q55" s="7"/>
     </row>
     <row r="56" spans="1:17" hidden="1">
-      <c r="A56" s="3"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="7"/>
       <c r="C56" s="7"/>
       <c r="D56" s="7"/>
@@ -2773,25 +2749,7 @@
       <c r="P56" s="7"/>
       <c r="Q56" s="7"/>
     </row>
-    <row r="57" spans="1:17" hidden="1">
-      <c r="A57" s="7"/>
-      <c r="B57" s="7"/>
-      <c r="C57" s="7"/>
-      <c r="D57" s="7"/>
-      <c r="E57" s="7"/>
-      <c r="F57" s="7"/>
-      <c r="G57" s="7"/>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-      <c r="K57" s="7"/>
-      <c r="L57" s="7"/>
-      <c r="M57" s="7"/>
-      <c r="N57" s="7"/>
-      <c r="O57" s="7"/>
-      <c r="P57" s="7"/>
-      <c r="Q57" s="7"/>
-    </row>
+    <row r="57" spans="1:17" ht="15" customHeight="1"/>
     <row r="58" spans="1:17" ht="15" customHeight="1"/>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -2895,18 +2853,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:C31">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="-4"/>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="4"/>
-        <color rgb="FFFFC000"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>
@@ -2919,7 +2865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
   <cols>

</xml_diff>

<commit_message>
fix(warns): Remove openpyxl warnings.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\compas.vinz\co2mpas\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="output_report" sheetId="6" r:id="rId1"/>
     <sheet name="dice_report" sheetId="4" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1320,7 +1315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1"/>
   <cols>

</xml_diff>

<commit_message>
fix(output_template): Remove warning unknown extension of openpyxl.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -2,42 +2,31 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16260"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="37395" windowHeight="16500"/>
   </bookViews>
   <sheets>
-    <sheet name="output_report" sheetId="6" r:id="rId1"/>
-    <sheet name="dice_report" sheetId="4" state="hidden" r:id="rId2"/>
+    <sheet name="output_report" sheetId="4" r:id="rId1"/>
+    <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="75">
   <si>
-    <t>Vehicle H</t>
-  </si>
-  <si>
-    <t>Vehicle L</t>
-  </si>
-  <si>
-    <t>units</t>
-  </si>
-  <si>
-    <t>cc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CO2MPAS deviation </t>
-  </si>
-  <si>
-    <t>%</t>
+    <t>Vehicle Family ID</t>
+  </si>
+  <si>
+    <t>CO2MPAS version</t>
+  </si>
+  <si>
+    <t>Date/Time</t>
+  </si>
+  <si>
+    <t>Type approval mode</t>
   </si>
   <si>
     <r>
@@ -68,6 +57,15 @@
     </r>
   </si>
   <si>
+    <t>Vehicle H</t>
+  </si>
+  <si>
+    <t>Vehicle L</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
     <r>
       <t>NEDC CO</t>
     </r>
@@ -102,6 +100,12 @@
     <t xml:space="preserve">NEDC CO2MPAS simulated </t>
   </si>
   <si>
+    <t xml:space="preserve">CO2MPAS deviation </t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
     <t>*Ki factor - corrected</t>
   </si>
   <si>
@@ -142,142 +146,6 @@
     <t>CO2MPAS simulated EUDC</t>
   </si>
   <si>
-    <t>NEDC Inputs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F0 </t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F1 </t>
-  </si>
-  <si>
-    <t>N/km/h</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F2 </t>
-  </si>
-  <si>
-    <r>
-      <t>N/(km/h)</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-  </si>
-  <si>
-    <t>Inertia</t>
-  </si>
-  <si>
-    <t>kg</t>
-  </si>
-  <si>
-    <t>WLTP Inputs</t>
-  </si>
-  <si>
-    <t>Test Mass</t>
-  </si>
-  <si>
-    <t>CO2 emission phase Low</t>
-  </si>
-  <si>
-    <t>CO2 emission phase Medium</t>
-  </si>
-  <si>
-    <t>CO2 emission phase High</t>
-  </si>
-  <si>
-    <t>CO2 emission phase Extra-High</t>
-  </si>
-  <si>
-    <t>Field</t>
-  </si>
-  <si>
-    <t>vehicle-H</t>
-  </si>
-  <si>
-    <t>vehicle-L</t>
-  </si>
-  <si>
-    <t>fuel_type</t>
-  </si>
-  <si>
-    <t>engine_capacity</t>
-  </si>
-  <si>
-    <t>gear_box_type</t>
-  </si>
-  <si>
-    <t>engine_is_turbo</t>
-  </si>
-  <si>
-    <t>vehicle_family_id</t>
-  </si>
-  <si>
-    <t>CO2MPAS_version</t>
-  </si>
-  <si>
-    <t>datetime</t>
-  </si>
-  <si>
-    <t>TA_mode</t>
-  </si>
-  <si>
-    <t>Vehicle</t>
-  </si>
-  <si>
-    <t>at_model</t>
-  </si>
-  <si>
-    <t>alternator_model</t>
-  </si>
-  <si>
-    <t>clutch_torque_converter_model</t>
-  </si>
-  <si>
-    <t>co2_params</t>
-  </si>
-  <si>
-    <t>engine_cold_start_speed_model</t>
-  </si>
-  <si>
-    <t>engine_coolant_temperature_model</t>
-  </si>
-  <si>
-    <t>engine_speed_model</t>
-  </si>
-  <si>
-    <t>start_stop_model</t>
-  </si>
-  <si>
-    <t>Model_scores</t>
-  </si>
-  <si>
-    <t>CO2MPAS_deviation</t>
-  </si>
-  <si>
-    <t>Vehicle Family ID</t>
-  </si>
-  <si>
-    <t>CO2MPAS version</t>
-  </si>
-  <si>
-    <t>Date/Time</t>
-  </si>
-  <si>
-    <t>Type approval mode</t>
-  </si>
-  <si>
     <t>Fuel Type</t>
   </si>
   <si>
@@ -285,6 +153,9 @@
   </si>
   <si>
     <t>Engine Capacity</t>
+  </si>
+  <si>
+    <t>cc</t>
   </si>
   <si>
     <t>Gearbox type</t>
@@ -350,10 +221,134 @@
     <t>start_stop_model score</t>
   </si>
   <si>
+    <t>NEDC Inputs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F0 </t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F1 </t>
+  </si>
+  <si>
+    <t>N/km/h</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F2 </t>
+  </si>
+  <si>
+    <r>
+      <t>N/(km/h)</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+  </si>
+  <si>
+    <t>Inertia</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>WLTP Inputs</t>
+  </si>
+  <si>
+    <t>Test Mass</t>
+  </si>
+  <si>
+    <t>CO2 emission phase Low</t>
+  </si>
+  <si>
+    <t>CO2 emission phase Medium</t>
+  </si>
+  <si>
+    <t>CO2 emission phase High</t>
+  </si>
+  <si>
+    <t>CO2 emission phase Extra-High</t>
+  </si>
+  <si>
+    <t>start_stop_model</t>
+  </si>
+  <si>
+    <t>engine_speed_model</t>
+  </si>
+  <si>
+    <t>engine_coolant_temperature_model</t>
+  </si>
+  <si>
+    <t>engine_cold_start_speed_model</t>
+  </si>
+  <si>
+    <t>co2_params</t>
+  </si>
+  <si>
+    <t>clutch_torque_converter_model</t>
+  </si>
+  <si>
+    <t>at_model</t>
+  </si>
+  <si>
+    <t>alternator_model</t>
+  </si>
+  <si>
+    <t>Model_scores</t>
+  </si>
+  <si>
+    <t>engine_is_turbo</t>
+  </si>
+  <si>
+    <t>gear_box_type</t>
+  </si>
+  <si>
+    <t>engine_capacity</t>
+  </si>
+  <si>
+    <t>fuel_type</t>
+  </si>
+  <si>
+    <t>Vehicle</t>
+  </si>
+  <si>
+    <t>CO2MPAS_deviation</t>
+  </si>
+  <si>
+    <t>TA_mode</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
     <t>dice_report</t>
   </si>
   <si>
     <t>report_type</t>
+  </si>
+  <si>
+    <t>CO2MPAS_version</t>
+  </si>
+  <si>
+    <t>vehicle_family_id</t>
+  </si>
+  <si>
+    <t>vehicle-L</t>
+  </si>
+  <si>
+    <t>vehicle-H</t>
+  </si>
+  <si>
+    <t>Field</t>
   </si>
 </sst>
 </file>
@@ -364,7 +359,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -397,16 +392,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <vertAlign val="subscript"/>
-      <sz val="11"/>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -417,20 +412,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <vertAlign val="superscript"/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -449,6 +430,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -777,19 +766,59 @@
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
       <protection hidden="1"/>
     </xf>
@@ -805,6 +834,90 @@
       <alignment horizontal="right" vertical="center"/>
       <protection hidden="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
@@ -825,143 +938,19 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="11" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="12" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="5" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="5" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="9" fillId="5" borderId="12" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="5" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
@@ -1019,9 +1008,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1069,12 +1055,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian Light"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -1104,12 +1090,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="Yu Gothic"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="DengXian"/>
+        <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -1330,7 +1316,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B1" s="2" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_vehicle_family_id_Value"),"")</f>
@@ -1354,7 +1340,7 @@
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_CO2MPAS_version_Value"),"")</f>
@@ -1378,7 +1364,7 @@
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_Simulation_started_Value"),"")</f>
@@ -1402,7 +1388,7 @@
     </row>
     <row r="4" spans="1:17" ht="15.75" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="B4" s="6" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_type_approval_mode_Value"),"")</f>
@@ -1463,17 +1449,17 @@
       <c r="Q6" s="7"/>
     </row>
     <row r="7" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="27" t="s">
-        <v>2</v>
+      <c r="D7" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -1490,19 +1476,19 @@
       <c r="Q7" s="7"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A8" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="29" t="str">
+      <c r="A8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="13" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_target_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C8" s="30" t="str">
+      <c r="C8" s="14" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_target_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D8" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -1519,19 +1505,19 @@
       <c r="Q8" s="7"/>
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="16" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
+        <v/>
+      </c>
+      <c r="C9" s="17" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
+        <v/>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" s="10" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_declared_co2_emission_declared_value__CO2g_km_"),"")</f>
-        <v/>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>8</v>
       </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -1548,19 +1534,19 @@
       <c r="Q9" s="7"/>
     </row>
     <row r="10" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="34" t="str">
+      <c r="A10" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="19" t="str">
         <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
         <v/>
       </c>
-      <c r="C10" s="35" t="str">
+      <c r="C10" s="20" t="str">
         <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100, "")</f>
         <v/>
       </c>
       <c r="D10" s="7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -1577,11 +1563,11 @@
       <c r="Q10" s="7"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A11" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="13"/>
+      <c r="A11" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="22"/>
+      <c r="C11" s="23"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -1599,13 +1585,13 @@
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
       <c r="A12" s="4"/>
-      <c r="B12" s="14"/>
+      <c r="B12" s="24"/>
       <c r="C12" s="3"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="36"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
@@ -1617,14 +1603,14 @@
       <c r="Q12" s="7"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A13" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>1</v>
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>6</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1642,19 +1628,19 @@
       <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A14" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="37" t="str">
+      <c r="A14" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="26" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_value__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C14" s="38" t="str">
+      <c r="C14" s="27" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_value__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D14" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -1671,19 +1657,19 @@
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A15" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="10" t="str">
+      <c r="A15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_UDC__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C15" s="32" t="str">
+      <c r="C15" s="17" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_UDC__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D15" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -1700,19 +1686,19 @@
       <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A16" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="39" t="str">
+      <c r="A16" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="28" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_co2_emission_EUDC__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C16" s="40" t="str">
+      <c r="C16" s="29" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_co2_emission_EUDC__CO2g_km_"),"")</f>
         <v/>
       </c>
       <c r="D16" s="7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -1729,9 +1715,9 @@
       <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A17" s="20"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -1748,15 +1734,15 @@
       <c r="Q17" s="7"/>
     </row>
     <row r="18" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A18" s="42"/>
-      <c r="B18" s="43" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="44" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>2</v>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -1773,19 +1759,19 @@
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A19" s="45" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="46" t="str">
+      <c r="A19" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19" s="36" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
         <v/>
       </c>
-      <c r="C19" s="47" t="str">
+      <c r="C19" s="37" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
         <v/>
       </c>
       <c r="D19" s="7" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1802,19 +1788,19 @@
       <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A20" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="8" t="str">
+      <c r="A20" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="38" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
         <v/>
       </c>
-      <c r="C20" s="48" t="str">
+      <c r="C20" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
         <v/>
       </c>
       <c r="D20" s="7" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -1831,19 +1817,19 @@
       <c r="Q20" s="7"/>
     </row>
     <row r="21" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A21" s="31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="8" t="str">
+      <c r="A21" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="38" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
-      <c r="C21" s="48" t="str">
+      <c r="C21" s="39" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
         <v/>
       </c>
       <c r="D21" s="7" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -1860,19 +1846,19 @@
       <c r="Q21" s="7"/>
     </row>
     <row r="22" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A22" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B22" s="49" t="str">
+      <c r="A22" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" s="40" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
         <v/>
       </c>
-      <c r="C22" s="50" t="str">
+      <c r="C22" s="41" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
         <v/>
       </c>
       <c r="D22" s="7" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -1889,19 +1875,19 @@
       <c r="Q22" s="7"/>
     </row>
     <row r="23" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A23" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="51" t="str">
+      <c r="A23" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C23" s="52" t="str">
+      <c r="C23" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D23" s="7" t="s">
-        <v>62</v>
+        <v>25</v>
       </c>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -1918,19 +1904,19 @@
       <c r="Q23" s="7"/>
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A24" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="51" t="str">
+      <c r="A24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C24" s="52" t="str">
+      <c r="C24" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D24" s="7" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -1947,19 +1933,19 @@
       <c r="Q24" s="7"/>
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A25" s="31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B25" s="51" t="str">
+      <c r="A25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C25" s="52" t="str">
+      <c r="C25" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D25" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -1976,19 +1962,19 @@
       <c r="Q25" s="7"/>
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A26" s="31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B26" s="51" t="str">
+      <c r="A26" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C26" s="52" t="str">
+      <c r="C26" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D26" s="7" t="s">
-        <v>67</v>
+        <v>30</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -2005,19 +1991,19 @@
       <c r="Q26" s="7"/>
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A27" s="31" t="s">
-        <v>68</v>
-      </c>
-      <c r="B27" s="51" t="str">
+      <c r="A27" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C27" s="52" t="str">
+      <c r="C27" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D27" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -2034,19 +2020,19 @@
       <c r="Q27" s="7"/>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A28" s="31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28" s="51" t="str">
+      <c r="A28" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C28" s="52" t="str">
+      <c r="C28" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D28" s="7" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -2063,19 +2049,19 @@
       <c r="Q28" s="7"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A29" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B29" s="51" t="str">
+      <c r="A29" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29" s="42" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C29" s="52" t="str">
+      <c r="C29" s="43" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D29" s="7" t="s">
-        <v>65</v>
+        <v>28</v>
       </c>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -2092,19 +2078,19 @@
       <c r="Q29" s="7"/>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A30" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="B30" s="53" t="str">
+      <c r="A30" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="44" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C30" s="54" t="str">
+      <c r="C30" s="45" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="D30" s="7" t="s">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -2122,7 +2108,7 @@
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
       <c r="A31" s="4"/>
-      <c r="B31" s="14"/>
+      <c r="B31" s="24"/>
       <c r="C31" s="3"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
@@ -2140,14 +2126,14 @@
       <c r="Q31" s="7"/>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A32" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="15" t="s">
-        <v>1</v>
+      <c r="A32" s="46" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="46" t="s">
+        <v>6</v>
       </c>
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
@@ -2165,19 +2151,19 @@
       <c r="Q32" s="7"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A33" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B33" s="10" t="str">
+      <c r="A33" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
-      <c r="C33" s="10" t="str">
+      <c r="C33" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
       <c r="D33" s="7" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -2194,19 +2180,19 @@
       <c r="Q33" s="7"/>
     </row>
     <row r="34" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A34" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B34" s="18" t="str">
+      <c r="A34" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B34" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
-      <c r="C34" s="18" t="str">
+      <c r="C34" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="D34" s="7" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -2223,19 +2209,19 @@
       <c r="Q34" s="7"/>
     </row>
     <row r="35" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A35" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="18" t="str">
+      <c r="A35" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
-      <c r="C35" s="18" t="str">
+      <c r="C35" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="D35" s="7" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -2252,19 +2238,19 @@
       <c r="Q35" s="7"/>
     </row>
     <row r="36" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A36" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" s="19" t="str">
+      <c r="A36" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="50" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="C36" s="19" t="str">
+      <c r="C36" s="50" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="D36" s="41" t="s">
-        <v>23</v>
+      <c r="D36" s="51" t="s">
+        <v>44</v>
       </c>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -2281,14 +2267,14 @@
       <c r="Q36" s="7"/>
     </row>
     <row r="37" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A37" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>1</v>
+      <c r="A37" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B37" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="46" t="s">
+        <v>6</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
@@ -2306,19 +2292,19 @@
       <c r="Q37" s="7"/>
     </row>
     <row r="38" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A38" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B38" s="10" t="str">
+      <c r="A38" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
-      <c r="C38" s="10" t="str">
+      <c r="C38" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f0__N_"),"")</f>
         <v/>
       </c>
       <c r="D38" s="7" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -2335,19 +2321,19 @@
       <c r="Q38" s="7"/>
     </row>
     <row r="39" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A39" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="18" t="str">
+      <c r="A39" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
-      <c r="C39" s="18" t="str">
+      <c r="C39" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f1__N__km_h__"),"")</f>
         <v/>
       </c>
       <c r="D39" s="7" t="s">
-        <v>19</v>
+        <v>40</v>
       </c>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -2364,19 +2350,19 @@
       <c r="Q39" s="7"/>
     </row>
     <row r="40" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A40" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="B40" s="18" t="str">
+      <c r="A40" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
-      <c r="C40" s="18" t="str">
+      <c r="C40" s="49" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_f2__N__km_h__2_"),"")</f>
         <v/>
       </c>
       <c r="D40" s="7" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -2393,19 +2379,19 @@
       <c r="Q40" s="7"/>
     </row>
     <row r="41" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A41" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="19" t="str">
+      <c r="A41" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="50" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="C41" s="19" t="str">
+      <c r="C41" s="50" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_vehicle_mass__kg_"),"")</f>
         <v/>
       </c>
-      <c r="D41" s="41" t="s">
-        <v>23</v>
+      <c r="D41" s="51" t="s">
+        <v>44</v>
       </c>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -2422,19 +2408,19 @@
       <c r="Q41" s="7"/>
     </row>
     <row r="42" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A42" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="10" t="str">
+      <c r="A42" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B42" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C42" s="10" t="str">
+      <c r="C42" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_low__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="D42" s="41" t="s">
-        <v>8</v>
+      <c r="D42" s="51" t="s">
+        <v>9</v>
       </c>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -2451,19 +2437,19 @@
       <c r="Q42" s="7"/>
     </row>
     <row r="43" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A43" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" s="10" t="str">
+      <c r="A43" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="B43" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C43" s="10" t="str">
+      <c r="C43" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_medium__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="D43" s="41" t="s">
-        <v>8</v>
+      <c r="D43" s="51" t="s">
+        <v>9</v>
       </c>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -2480,19 +2466,19 @@
       <c r="Q43" s="7"/>
     </row>
     <row r="44" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A44" s="16" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" s="10" t="str">
+      <c r="A44" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C44" s="10" t="str">
+      <c r="C44" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="D44" s="41" t="s">
-        <v>8</v>
+      <c r="D44" s="51" t="s">
+        <v>9</v>
       </c>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -2509,19 +2495,19 @@
       <c r="Q44" s="7"/>
     </row>
     <row r="45" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A45" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="B45" s="10" t="str">
+      <c r="A45" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_h_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="C45" s="10" t="str">
+      <c r="C45" s="16" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_results_wltp_l_calibration_output_co2_emission_extra_high__CO2g_km_"),"")</f>
         <v/>
       </c>
-      <c r="D45" s="41" t="s">
-        <v>8</v>
+      <c r="D45" s="51" t="s">
+        <v>9</v>
       </c>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -2751,7 +2737,7 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="B10:C10">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -2763,15 +2749,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4">
-    <cfRule type="expression" dxfId="5" priority="19">
+    <cfRule type="expression" dxfId="5" priority="9">
       <formula>$B$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="20">
+    <cfRule type="expression" dxfId="4" priority="10">
       <formula>$B$4="True"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B23:C23">
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -2781,7 +2767,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24:C24">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -2791,7 +2777,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:C25">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -2801,7 +2787,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:C26">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -2811,7 +2797,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B27:C27">
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -2821,7 +2807,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28:C28">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -2831,7 +2817,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:C29">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -2841,7 +2827,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30:C30">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -2862,29 +2848,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="27.140625" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="11.85546875" style="9"/>
+    <col min="1" max="1" width="34.5703125" style="52" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="27.140625" style="52" customWidth="1"/>
+    <col min="4" max="16384" width="11.85546875" style="52"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A1" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="22" t="s">
-        <v>32</v>
+      <c r="A1" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="53" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="5" customFormat="1" ht="15">
       <c r="A2" s="1" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B2" s="2" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_vehicle_family_id_Value"),"")</f>
@@ -2897,7 +2885,7 @@
     </row>
     <row r="3" spans="1:3" s="5" customFormat="1" ht="15">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>70</v>
       </c>
       <c r="B3" s="2" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_CO2MPAS_version_Value"),"")</f>
@@ -2910,16 +2898,16 @@
     </row>
     <row r="4" spans="1:3" s="5" customFormat="1" ht="15">
       <c r="A4" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" s="5" customFormat="1" ht="15">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B5" s="2" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_Simulation_started_Value"),"")</f>
@@ -2932,7 +2920,7 @@
     </row>
     <row r="6" spans="1:3" s="5" customFormat="1" ht="15">
       <c r="A6" s="1" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B6" s="6" t="str">
         <f ca="1">IFERROR(INDIRECT("summary!_info_type_approval_mode_Value"),"")</f>
@@ -2944,193 +2932,192 @@
       </c>
     </row>
     <row r="7" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="54" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="54" t="str">
+        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
+        <v/>
+      </c>
+      <c r="C7" s="54" t="str">
+        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A8" s="53" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="53"/>
+    </row>
+    <row r="9" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A9" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
+        <v/>
+      </c>
+      <c r="C9" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A10" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
+        <v/>
+      </c>
+      <c r="C10" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A11" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
+        <v/>
+      </c>
+      <c r="C11" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A12" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+        <v/>
+      </c>
+      <c r="C12" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A13" s="53" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="53"/>
+      <c r="C13" s="53"/>
+    </row>
+    <row r="14" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A14" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C14" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A15" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C15" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A16" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C16" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A17" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C17" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A18" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C18" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="19" spans="1:3" s="5" customFormat="1" ht="15">
+      <c r="A19" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C19" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="15">
+      <c r="A20" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="C20" s="38" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15">
+      <c r="A21" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="23" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_h_prediction_target_ratio")-1)*100,"")</f>
-        <v/>
-      </c>
-      <c r="C7" s="23" t="str">
-        <f ca="1">IFERROR((INDIRECT("summary!_comparison_declared_co2_emission_value_prediction_nedc_l_prediction_target_ratio")-1)*100,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A8" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-    </row>
-    <row r="9" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A9" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_fuel_type__"),"")</f>
-        <v/>
-      </c>
-      <c r="C9" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_fuel_type__"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A10" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="B10" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
-        <v/>
-      </c>
-      <c r="C10" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_capacity__cm3_"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A11" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B11" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_gear_box_type__"),"")</f>
-        <v/>
-      </c>
-      <c r="C11" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_gear_box_type__"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A12" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B12" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_h_prediction_output_vehicle_engine_is_turbo__"),"")</f>
-        <v/>
-      </c>
-      <c r="C12" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("summary!_results_nedc_l_prediction_output_vehicle_engine_is_turbo__"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A13" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-    </row>
-    <row r="14" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A14" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C14" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_alternator_model_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A15" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C15" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_at_model_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A16" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="B16" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C16" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_clutch_torque_converter_model_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A17" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C17" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_co2_params_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A18" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C18" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_cold_start_speed_model_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="5" customFormat="1" ht="15">
-      <c r="A19" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C19" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_coolant_temperature_model_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="15">
-      <c r="A20" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="C20" s="8" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_engine_speed_model_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="15">
-      <c r="A21" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="B21" s="8" t="str">
+      <c r="B21" s="38" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_h_score"),"")</f>
         <v/>
       </c>
-      <c r="C21" s="8" t="str">
+      <c r="C21" s="38" t="str">
         <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_score_by_model_start_stop_model_wltp_l_score"),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
-  <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="B7:C7">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -3142,15 +3129,15 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="3" priority="13">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$B$6="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="14">
+    <cfRule type="expression" dxfId="2" priority="5">
       <formula>$B$6="True"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -3174,10 +3161,5 @@
   <headerFooter>
     <oddHeader>&amp;CCO2MPAS DICE REPORT</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(thermal), #459: Split thermal model error coefficient as cold and hot.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7332B1B9-3A44-FD45-83C0-17A1C49DFEED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="16755"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
     <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -437,11 +443,17 @@
   <si>
     <t>Model_scores WLTP-L</t>
   </si>
+  <si>
+    <t>engine_coolant_temperature_model (cold)</t>
+  </si>
+  <si>
+    <t>engine_coolant_temperature_model (hot)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1316,6 +1328,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1363,7 +1378,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1396,9 +1411,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1431,6 +1463,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1606,29 +1655,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B1:B2"/>
-    </sheetView>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="1.1640625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
     <col min="4" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
-    <col min="8" max="8" width="1.140625" style="54" customWidth="1"/>
-    <col min="9" max="9" width="1.140625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="1.1640625" style="54" customWidth="1"/>
+    <col min="9" max="9" width="1.1640625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.33203125" style="3" customWidth="1"/>
     <col min="12" max="15" width="12" style="3" customWidth="1"/>
-    <col min="16" max="16" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.140625" style="10" customWidth="1"/>
-    <col min="18" max="16384" width="8.85546875" style="3" hidden="1"/>
+    <col min="16" max="16" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.1640625" style="10" customWidth="1"/>
+    <col min="18" max="16384" width="8.83203125" style="3" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" customHeight="1">
@@ -2121,7 +2168,7 @@
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
     </row>
-    <row r="16" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
+    <row r="16" spans="2:21" ht="15.75" customHeight="1">
       <c r="B16" s="61" t="s">
         <v>69</v>
       </c>
@@ -2139,24 +2186,24 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
-      <c r="J16" s="75" t="s">
-        <v>24</v>
-      </c>
-      <c r="K16" s="76"/>
-      <c r="L16" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M16" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N16" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O16" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_l_score"),"")</f>
+      <c r="J16" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="K16" s="73"/>
+      <c r="L16" s="23" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M16" s="24" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N16" s="23" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O16" s="24" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P16" s="19" t="s">
@@ -2185,63 +2232,63 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="10"/>
-      <c r="J17" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="K17" s="76"/>
-      <c r="L17" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M17" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N17" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O17" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
+      <c r="J17" s="65" t="s">
+        <v>78</v>
+      </c>
+      <c r="K17" s="74"/>
+      <c r="L17" s="40" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M17" s="41" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N17" s="40" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O17" s="41" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P17" s="19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="2:21" ht="15.75" customHeight="1">
+    <row r="18" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
       <c r="E18" s="39"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="10"/>
-      <c r="J18" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="K18" s="73"/>
-      <c r="L18" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M18" s="24" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N18" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O18" s="24" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
+      <c r="J18" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18" s="76"/>
+      <c r="L18" s="31" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M18" s="32" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N18" s="31" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O18" s="32" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P18" s="19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
@@ -2259,24 +2306,24 @@
       <c r="G19" s="68"/>
       <c r="H19" s="12"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="K19" s="74"/>
-      <c r="L19" s="40" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M19" s="41" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N19" s="40" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O19" s="41" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
+      <c r="J19" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="73"/>
+      <c r="L19" s="23" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M19" s="24" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N19" s="23" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O19" s="24" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P19" s="19" t="s">
@@ -2291,7 +2338,29 @@
     <row r="20" spans="2:21" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="G20" s="9"/>
       <c r="H20" s="10"/>
-      <c r="J20" s="9"/>
+      <c r="J20" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="74"/>
+      <c r="L20" s="40" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M20" s="41" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N20" s="40" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O20" s="41" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="P20" s="19" t="s">
+        <v>18</v>
+      </c>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
@@ -3023,9 +3092,8 @@
       <c r="U60" s="9"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D11:E11">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -3037,7 +3105,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3047,7 +3115,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3057,7 +3125,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3067,7 +3135,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="43">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3077,7 +3145,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3087,7 +3155,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="colorScale" priority="36">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3097,7 +3165,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3107,7 +3175,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3116,8 +3184,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="colorScale" priority="33">
+  <conditionalFormatting sqref="L18">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3126,8 +3194,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
-    <cfRule type="colorScale" priority="32">
+  <conditionalFormatting sqref="L20">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3137,7 +3205,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3147,7 +3215,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3157,7 +3225,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3167,7 +3235,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3177,7 +3245,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3187,7 +3255,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3197,7 +3265,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3207,7 +3275,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3217,7 +3285,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3227,7 +3295,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3237,7 +3305,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3247,7 +3315,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3257,7 +3325,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3267,7 +3335,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3277,7 +3345,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3287,7 +3355,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3297,7 +3365,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3307,7 +3375,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3317,7 +3385,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3327,7 +3395,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3336,8 +3404,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="M18">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3346,8 +3414,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N17">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="N18">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3356,8 +3424,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O17">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="O18">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3366,8 +3434,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="L19">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3376,8 +3444,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M18">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="M19">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3386,8 +3454,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="N19">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3396,8 +3464,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="O19">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3406,8 +3474,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="M20">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3416,8 +3484,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="N20">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3426,8 +3494,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O19">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="O20">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3437,11 +3505,51 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4 K4">
-    <cfRule type="expression" dxfId="1" priority="42">
+    <cfRule type="expression" dxfId="1" priority="46">
       <formula>$C$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="43">
+    <cfRule type="expression" dxfId="0" priority="47">
       <formula>$C$4="True"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L17">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O17">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="3"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFC000"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3454,18 +3562,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.5703125" style="58" customWidth="1"/>
+    <col min="1" max="1" width="34.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.5" style="58" customWidth="1"/>
     <col min="4" max="4" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.85546875" style="58"/>
+    <col min="5" max="5" width="7.5" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.83203125" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="15">

</xml_diff>

<commit_message>
refact(selector): Revert split of thermal model error coefficient.
</commit_message>
<xml_diff>
--- a/co2mpas/co2mpas_output_template.xlsx
+++ b/co2mpas/co2mpas_output_template.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincenzoarcidiacono/PycharmProjects/co2mpas/co2mpas/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7332B1B9-3A44-FD45-83C0-17A1C49DFEED}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="37395" windowHeight="16755"/>
   </bookViews>
   <sheets>
     <sheet name="output_report" sheetId="4" r:id="rId1"/>
     <sheet name="dice_report" sheetId="5" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="77">
   <si>
     <t>Vehicle Family ID</t>
   </si>
@@ -443,17 +437,11 @@
   <si>
     <t>Model_scores WLTP-L</t>
   </si>
-  <si>
-    <t>engine_coolant_temperature_model (cold)</t>
-  </si>
-  <si>
-    <t>engine_coolant_temperature_model (hot)</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -1328,9 +1316,6 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1378,7 +1363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1411,26 +1396,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1463,23 +1431,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1655,27 +1606,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U60"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0"/>
+    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" showRuler="0" view="pageLayout" workbookViewId="0">
+      <selection activeCell="B2" sqref="B1:B2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="0" customHeight="1" zeroHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.1640625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="1.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.28515625" style="3" customWidth="1"/>
     <col min="4" max="5" width="12" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="1.1640625" style="54" customWidth="1"/>
-    <col min="9" max="9" width="1.1640625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="1.140625" style="54" customWidth="1"/>
+    <col min="9" max="9" width="1.140625" style="10" customWidth="1"/>
+    <col min="10" max="10" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.28515625" style="3" customWidth="1"/>
     <col min="12" max="15" width="12" style="3" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="1.1640625" style="10" customWidth="1"/>
-    <col min="18" max="16384" width="8.83203125" style="3" hidden="1"/>
+    <col min="16" max="16" width="7.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="1.140625" style="10" customWidth="1"/>
+    <col min="18" max="16384" width="8.85546875" style="3" hidden="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:21" ht="15.75" customHeight="1">
@@ -2168,7 +2121,7 @@
       <c r="T15" s="9"/>
       <c r="U15" s="9"/>
     </row>
-    <row r="16" spans="2:21" ht="15.75" customHeight="1">
+    <row r="16" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
       <c r="B16" s="61" t="s">
         <v>69</v>
       </c>
@@ -2186,24 +2139,24 @@
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="10"/>
-      <c r="J16" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="K16" s="73"/>
-      <c r="L16" s="23" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M16" s="24" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N16" s="23" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O16" s="24" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_cold_wltp_l_wltp_l_score"),"")</f>
+      <c r="J16" s="75" t="s">
+        <v>24</v>
+      </c>
+      <c r="K16" s="76"/>
+      <c r="L16" s="31" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M16" s="32" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N16" s="31" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O16" s="32" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_engine_coolant_temperatures_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P16" s="19" t="s">
@@ -2232,63 +2185,63 @@
       </c>
       <c r="G17" s="9"/>
       <c r="H17" s="10"/>
-      <c r="J17" s="65" t="s">
-        <v>78</v>
-      </c>
-      <c r="K17" s="74"/>
-      <c r="L17" s="40" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M17" s="41" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N17" s="40" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O17" s="41" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_coolant_temperature_model_hot_wltp_l_wltp_l_score"),"")</f>
+      <c r="J17" s="75" t="s">
+        <v>26</v>
+      </c>
+      <c r="K17" s="76"/>
+      <c r="L17" s="31" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M17" s="32" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N17" s="31" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O17" s="32" t="str">
+        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P17" s="19" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="9"/>
       <c r="U17" s="9"/>
     </row>
-    <row r="18" spans="2:21" ht="15.75" customHeight="1" thickBot="1">
+    <row r="18" spans="2:21" ht="15.75" customHeight="1">
       <c r="C18" s="38"/>
       <c r="D18" s="39"/>
       <c r="E18" s="39"/>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
       <c r="H18" s="10"/>
-      <c r="J18" s="75" t="s">
-        <v>26</v>
-      </c>
-      <c r="K18" s="76"/>
-      <c r="L18" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M18" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N18" s="31" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O18" s="32" t="str">
-        <f ca="1">IFERROR(INDIRECT("data.calibration.model_scores!_scores_engine_speed_model_engine_speeds_out_wltp_l_wltp_l_score"),"")</f>
+      <c r="J18" s="59" t="s">
+        <v>27</v>
+      </c>
+      <c r="K18" s="73"/>
+      <c r="L18" s="23" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M18" s="24" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N18" s="23" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O18" s="24" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P18" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
@@ -2306,24 +2259,24 @@
       <c r="G19" s="68"/>
       <c r="H19" s="12"/>
       <c r="I19" s="7"/>
-      <c r="J19" s="59" t="s">
-        <v>27</v>
-      </c>
-      <c r="K19" s="73"/>
-      <c r="L19" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M19" s="24" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N19" s="23" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O19" s="24" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_engine_starts_wltp_l_wltp_l_score"),"")</f>
+      <c r="J19" s="65" t="s">
+        <v>29</v>
+      </c>
+      <c r="K19" s="74"/>
+      <c r="L19" s="40" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="M19" s="41" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
+        <v/>
+      </c>
+      <c r="N19" s="40" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
+        <v/>
+      </c>
+      <c r="O19" s="41" t="str">
+        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
         <v/>
       </c>
       <c r="P19" s="19" t="s">
@@ -2338,29 +2291,7 @@
     <row r="20" spans="2:21" ht="15.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="G20" s="9"/>
       <c r="H20" s="10"/>
-      <c r="J20" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="K20" s="74"/>
-      <c r="L20" s="40" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="M20" s="41" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_h_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="N20" s="40" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_h_score"),"")</f>
-        <v/>
-      </c>
-      <c r="O20" s="41" t="str">
-        <f ca="1">IFERROR(-INDIRECT("data.calibration.model_scores!_scores_start_stop_model_on_engine_wltp_l_wltp_l_score"),"")</f>
-        <v/>
-      </c>
-      <c r="P20" s="19" t="s">
-        <v>18</v>
-      </c>
+      <c r="J20" s="9"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
       <c r="T20" s="9"/>
@@ -3092,8 +3023,9 @@
       <c r="U60" s="9"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <conditionalFormatting sqref="D11:E11">
-    <cfRule type="colorScale" priority="45">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="num" val="-4"/>
         <cfvo type="num" val="0"/>
@@ -3105,7 +3037,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3115,7 +3047,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3125,7 +3057,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O10">
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3135,7 +3067,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L11">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3145,7 +3077,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L13">
-    <cfRule type="colorScale" priority="41">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3155,7 +3087,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="colorScale" priority="40">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3165,7 +3097,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L15">
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3175,7 +3107,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3184,8 +3116,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L18">
-    <cfRule type="colorScale" priority="37">
+  <conditionalFormatting sqref="L17">
+    <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3194,8 +3126,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L20">
-    <cfRule type="colorScale" priority="36">
+  <conditionalFormatting sqref="L19">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3205,7 +3137,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3215,7 +3147,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O12">
-    <cfRule type="colorScale" priority="26">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3225,7 +3157,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3235,7 +3167,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3245,7 +3177,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N11">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3255,7 +3187,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N10">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3265,7 +3197,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O11">
-    <cfRule type="colorScale" priority="30">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="60"/>
@@ -3275,7 +3207,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3285,7 +3217,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N12">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="0"/>
@@ -3295,7 +3227,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O13">
-    <cfRule type="colorScale" priority="25">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3305,7 +3237,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N13">
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3315,7 +3247,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3325,7 +3257,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N14">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3335,7 +3267,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O14">
-    <cfRule type="colorScale" priority="21">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="0.5"/>
@@ -3345,7 +3277,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="colorScale" priority="20">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3355,7 +3287,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15">
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3365,7 +3297,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O15">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="100"/>
@@ -3375,7 +3307,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3385,7 +3317,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N16">
-    <cfRule type="colorScale" priority="16">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3395,7 +3327,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O16">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="3"/>
@@ -3404,8 +3336,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M18">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="M17">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3414,8 +3346,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N18">
-    <cfRule type="colorScale" priority="13">
+  <conditionalFormatting sqref="N17">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3424,8 +3356,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O18">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="O17">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="40"/>
@@ -3434,8 +3366,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L19">
-    <cfRule type="colorScale" priority="11">
+  <conditionalFormatting sqref="L18">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3444,8 +3376,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M19">
-    <cfRule type="colorScale" priority="10">
+  <conditionalFormatting sqref="M18">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3454,8 +3386,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N19">
-    <cfRule type="colorScale" priority="9">
+  <conditionalFormatting sqref="N18">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3464,8 +3396,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O19">
-    <cfRule type="colorScale" priority="8">
+  <conditionalFormatting sqref="O18">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3474,8 +3406,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M20">
-    <cfRule type="colorScale" priority="7">
+  <conditionalFormatting sqref="M19">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3484,8 +3416,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N20">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="N19">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3494,8 +3426,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O20">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="O19">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="-1"/>
         <cfvo type="num" val="-0.7"/>
@@ -3505,51 +3437,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4 K4">
-    <cfRule type="expression" dxfId="1" priority="46">
+    <cfRule type="expression" dxfId="1" priority="42">
       <formula>$C$4="False"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="47">
+    <cfRule type="expression" dxfId="0" priority="43">
       <formula>$C$4="True"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L17">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M17">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="N17">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="O17">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="3"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFC000"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3562,18 +3454,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C34"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" showRuler="0" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="34.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="22.5" style="58" customWidth="1"/>
+    <col min="1" max="1" width="34.42578125" style="58" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="22.5703125" style="58" customWidth="1"/>
     <col min="4" max="4" width="8" style="58" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5" style="58" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="11.83203125" style="58"/>
+    <col min="5" max="5" width="7.5703125" style="58" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="11.85546875" style="58"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" ht="15">

</xml_diff>